<commit_message>
Add dbc for SavvyCAN
</commit_message>
<xml_diff>
--- a/design/ND MX-5 CAN Decoding.xlsx
+++ b/design/ND MX-5 CAN Decoding.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\HavirNAS\Documents\Tomek\pojazdy\Miata30\KnurDash\KnurDashGit\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\KnurDash\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8F654B-CB5D-4443-8E13-D7EF75EFEFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AE6C61-F863-4263-9565-E84DB710D11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,6 +79,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 Offset:
@@ -101,6 +102,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Offset: 0
 Scaling: (1/160) MPH</t>
@@ -144,6 +146,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Neutral: 22 (dec)
 Clutch-in: 25 (dec)
@@ -166,6 +169,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Neutral/1st: 19 (dec)
 2nd: 11(dec)
@@ -190,6 +194,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Treat as signed integer
 Scaling: (-100/12750)+255 </t>
@@ -259,6 +264,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Offset: 32512
 Scaling:  Ref Vehicle Speed</t>
@@ -280,6 +286,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Offset: 32512
 Scaling:  Ref Vehicle Speed</t>
@@ -301,6 +308,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Offset: 32512
 Scaling: Ref Vehicle Speed</t>
@@ -322,6 +330,7 @@
         <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Offset: 32512
 Scaling:  Ref Vehicle Speed</t>
@@ -537,16 +546,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -557,10 +570,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1105,8 +1114,8 @@
   </sheetPr>
   <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1224,18 +1233,18 @@
         <f>HEX2DEC(C7)</f>
         <v>514</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="21"/>
+      <c r="G7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20" t="s">
+      <c r="H7" s="21"/>
+      <c r="I7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="19"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
@@ -1271,7 +1280,7 @@
       <c r="C10" s="13"/>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1282,10 +1291,10 @@
         <f>HEX2DEC(C11)</f>
         <v>576</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C12" s="13"/>
@@ -1302,10 +1311,10 @@
         <f>HEX2DEC(C13)</f>
         <v>120</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="15"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C14" s="13"/>
@@ -1322,22 +1331,22 @@
         <f>HEX2DEC(C15)</f>
         <v>533</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="16" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="17"/>
-      <c r="I15" s="16" t="s">
+      <c r="H15" s="15"/>
+      <c r="I15" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="16" t="s">
+      <c r="J15" s="15"/>
+      <c r="K15" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="17"/>
+      <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C16" s="13"/>
@@ -1351,13 +1360,13 @@
         <v>86</v>
       </c>
       <c r="D17" s="12">
-        <f t="shared" ref="D17:D19" si="0">HEX2DEC(C17)</f>
+        <f t="shared" ref="D17" si="0">HEX2DEC(C17)</f>
         <v>134</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="15"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
@@ -1405,22 +1414,22 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="23" t="str">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="19" t="str">
         <f>HYPERLINK("https://drive.google.com/open?id=15iy2YZ649EJ6RIQSPAJwfBqKBYgafXnz","Download link for RaceCaptureSettings")</f>
         <v>Download link for RaceCaptureSettings</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
       <c r="H25" s="3"/>
     </row>
     <row r="43" spans="2:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -1595,18 +1604,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="B24:D25"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update CAN frames definitions
</commit_message>
<xml_diff>
--- a/design/ND MX-5 CAN Decoding.xlsx
+++ b/design/ND MX-5 CAN Decoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\KnurDash\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCA70FA-A286-43AC-9A05-5C25376F051D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48711059-E928-448E-8C8A-3397FA5A0595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Notes:
 * All bytes are big-endian.</t>
@@ -291,10 +291,6 @@
     </r>
   </si>
   <si>
-    <t>offset 4 ?
-(mask 00010000)</t>
-  </si>
-  <si>
     <t>CAN mapping for Auto Sport Labs RaceCapture</t>
   </si>
   <si>
@@ -320,10 +316,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>Engine Coolant temp
-+40</t>
   </si>
   <si>
     <r>
@@ -383,13 +375,27 @@
 Offset:
 Scaling: 0.25</t>
     </r>
+  </si>
+  <si>
+    <t>4FA</t>
+  </si>
+  <si>
+    <t>IntakeAirTemp C
+offset: -40</t>
+  </si>
+  <si>
+    <t>https://github.com/timurrrr/RaceChronoDiyBleDevice/blob/master/can_db/mazda_mx5_nd.md</t>
+  </si>
+  <si>
+    <t>EngCoolantTemp
+offset: -40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -428,6 +434,13 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -470,10 +483,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -505,13 +519,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -523,19 +546,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,18 +574,18 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>962025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3333750" cy="5429250"/>
+    <xdr:ext cx="6000750" cy="2257425"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image2.png" title="Image">
+        <xdr:cNvPr id="6" name="image4.png" title="Image">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -587,157 +606,17 @@
     </xdr:pic>
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3486150" cy="5705475"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image5.png" title="Image">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5400675" cy="2886075"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="image3.png" title="Image">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14963775" y="5972175"/>
-          <a:ext cx="5400675" cy="2886075"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5191125" cy="5705475"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="image1.png" title="Image">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>962025</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6000750" cy="2257425"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="image4.png" title="Image">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>40560</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>477552</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:colOff>296577</xdr:colOff>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>190948</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -754,7 +633,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1074,17 +953,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:L51"/>
+  <dimension ref="B2:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="11" max="11" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1095,28 +976,28 @@
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
@@ -1184,7 +1065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1195,268 +1076,253 @@
         <f>HEX2DEC(C7)</f>
         <v>514</v>
       </c>
-      <c r="E7" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="23" t="s">
+      <c r="E7" s="14" t="s">
         <v>34</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="7"/>
       <c r="L7" s="7"/>
     </row>
-    <row r="8" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C8" s="13"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="2:12" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11">
+        <v>165</v>
+      </c>
+      <c r="D8" s="12">
+        <f>HEX2DEC(C8)</f>
+        <v>357</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="11">
-        <v>165</v>
+        <v>240</v>
       </c>
       <c r="D9" s="12">
         <f>HEX2DEC(C9)</f>
-        <v>357</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C10" s="13"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="11" spans="2:12" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>576</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="2:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="11">
+        <v>78</v>
+      </c>
+      <c r="D10" s="12">
+        <f>HEX2DEC(C10)</f>
+        <v>120</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="20"/>
+    </row>
+    <row r="11" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="11">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="D11" s="12">
         <f>HEX2DEC(C11)</f>
-        <v>576</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C12" s="13"/>
-      <c r="D12" s="12"/>
-    </row>
-    <row r="13" spans="2:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>533</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="17"/>
+      <c r="G11" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="11">
+        <v>86</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" ref="D12" si="0">HEX2DEC(C12)</f>
+        <v>134</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="20"/>
+    </row>
+    <row r="13" spans="2:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="11">
-        <v>78</v>
+        <v>420</v>
       </c>
       <c r="D13" s="12">
         <f>HEX2DEC(C13)</f>
-        <v>120</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="17"/>
-    </row>
-    <row r="14" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C14" s="13"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+        <v>1056</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="2:12" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="11">
-        <v>215</v>
-      </c>
-      <c r="D15" s="12">
-        <f>HEX2DEC(C15)</f>
-        <v>533</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="15"/>
-      <c r="I15" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="15"/>
+      <c r="C14" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="12">
+        <f>HEX2DEC(C14)</f>
+        <v>1274</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C16" s="13"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="11">
-        <v>86</v>
-      </c>
-      <c r="D17" s="12">
-        <f t="shared" ref="D17" si="0">HEX2DEC(C17)</f>
-        <v>134</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="17"/>
-    </row>
-    <row r="18" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="11">
-        <v>420</v>
-      </c>
-      <c r="D19" s="12">
-        <f>HEX2DEC(C19)</f>
-        <v>1056</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:12" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="11">
-        <v>415</v>
-      </c>
-      <c r="D21" s="12">
-        <f>HEX2DEC(C21)</f>
-        <v>1045</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="H21" s="6" t="s">
+      <c r="E16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E22" s="3"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E23" s="3"/>
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-    </row>
-    <row r="25" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="19" t="str">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+    </row>
+    <row r="18" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="22" t="str">
         <f>HYPERLINK("https://drive.google.com/open?id=15iy2YZ649EJ6RIQSPAJwfBqKBYgafXnz","Download link for RaceCaptureSettings")</f>
         <v>Download link for RaceCaptureSettings</v>
       </c>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="43" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="5"/>
+    </row>
+    <row r="38" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="5"/>
+    </row>
+    <row r="42" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="3"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="5"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B43" s="3"/>
       <c r="C43" s="5"/>
       <c r="D43" s="3"/>
       <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B44" s="3"/>
       <c r="C44" s="5"/>
       <c r="D44" s="3"/>
       <c r="E44" s="5"/>
     </row>
-    <row r="45" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B45" s="3"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B46" s="3"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="5"/>
-    </row>
-    <row r="47" spans="2:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="3"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="5"/>
-    </row>
-    <row r="49" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B49" s="3"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="5"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B50" s="3"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="5"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B51" s="3"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="5"/>
-    </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B17:D18"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="E11:F11"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="G7:H7"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B24:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I18" r:id="rId1" xr:uid="{282B1545-6CBF-4134-8F1B-70EB8ACD4C7D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
working on CAN decoding
</commit_message>
<xml_diff>
--- a/design/ND MX-5 CAN Decoding.xlsx
+++ b/design/ND MX-5 CAN Decoding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_git\KnurDash\design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48711059-E928-448E-8C8A-3397FA5A0595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E262A5A-F0D5-4691-9CBE-4AFC9668F55F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2025" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
   <si>
     <t>Notes:
 * All bytes are big-endian.</t>
@@ -120,28 +120,6 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Steering Torque candidate
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Treat as signed integer
-Scaling: (-100/12750)+255 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve">BrakePressure
 </t>
     </r>
@@ -389,13 +367,38 @@
   <si>
     <t>EngCoolantTemp
 offset: -40</t>
+  </si>
+  <si>
+    <t>verified on 2019 ND AE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Steering Torque candidate
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Treat as signed integer
+Scaling: (-100/12750)+255</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -444,8 +447,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +466,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -487,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -519,22 +535,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -546,12 +554,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -956,7 +980,7 @@
   <dimension ref="B2:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10:J10"/>
+      <selection activeCell="E11" sqref="E11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -973,31 +997,35 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="E2" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="25"/>
     </row>
     <row r="4" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="G4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
@@ -1076,16 +1104,16 @@
         <f>HEX2DEC(C7)</f>
         <v>514</v>
       </c>
-      <c r="E7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="14" t="s">
+      <c r="E7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="13" t="s">
+      <c r="F7" s="24"/>
+      <c r="G7" s="21" t="s">
         <v>32</v>
+      </c>
+      <c r="H7" s="22"/>
+      <c r="I7" s="27" t="s">
+        <v>31</v>
       </c>
       <c r="J7" s="8"/>
       <c r="K7" s="7"/>
@@ -1126,10 +1154,10 @@
         <f>HEX2DEC(C9)</f>
         <v>576</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="17"/>
+      <c r="E9" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="2:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
@@ -1142,10 +1170,10 @@
         <f>HEX2DEC(C10)</f>
         <v>120</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="20"/>
+      <c r="I10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="18"/>
     </row>
     <row r="11" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
@@ -1158,22 +1186,22 @@
         <f>HEX2DEC(C11)</f>
         <v>533</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="16"/>
+      <c r="G11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18" t="s">
+      <c r="H11" s="16"/>
+      <c r="I11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="17"/>
-      <c r="I11" s="18" t="s">
+      <c r="J11" s="16"/>
+      <c r="K11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="17"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
@@ -1186,10 +1214,10 @@
         <f t="shared" ref="D12" si="0">HEX2DEC(C12)</f>
         <v>134</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="20"/>
+      <c r="E12" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="2:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
@@ -1202,8 +1230,8 @@
         <f>HEX2DEC(C13)</f>
         <v>1056</v>
       </c>
-      <c r="E13" s="6" t="s">
-        <v>38</v>
+      <c r="E13" s="28" t="s">
+        <v>37</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1212,8 +1240,8 @@
       <c r="B14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="23" t="s">
-        <v>35</v>
+      <c r="C14" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="D14" s="12">
         <f>HEX2DEC(C14)</f>
@@ -1221,8 +1249,8 @@
       </c>
       <c r="E14" s="3"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="24" t="s">
-        <v>36</v>
+      <c r="I14" s="29" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="12.75" x14ac:dyDescent="0.2">
@@ -1234,25 +1262,25 @@
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="B17" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="2:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="22" t="str">
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="20" t="str">
         <f>HYPERLINK("https://drive.google.com/open?id=15iy2YZ649EJ6RIQSPAJwfBqKBYgafXnz","Download link for RaceCaptureSettings")</f>
         <v>Download link for RaceCaptureSettings</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="25" t="s">
-        <v>37</v>
+      <c r="I18" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -1307,17 +1335,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="B17:D18"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I18" r:id="rId1" xr:uid="{282B1545-6CBF-4134-8F1B-70EB8ACD4C7D}"/>

</xml_diff>